<commit_message>
method reverseWord(string s, int length)
</commit_message>
<xml_diff>
--- a/Прочие файлы/Протокол общий.xlsx
+++ b/Прочие файлы/Протокол общий.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StendLoRa\stend\Прочие файлы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Иван\Desktop\Test\Прочие файлы\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2ADC26-7A79-487A-94ED-C4D565A01843}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Протокол №__" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5207" uniqueCount="897">
   <si>
     <t>№ п/п</t>
   </si>
@@ -3372,12 +3373,18 @@
   </si>
   <si>
     <t>43</t>
+  </si>
+  <si>
+    <t>2800000816</t>
+  </si>
+  <si>
+    <t>2800000814</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3395,18 +3402,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="17">
@@ -3744,21 +3745,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -3794,6 +3780,21 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4079,12 +4080,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:T225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A226" sqref="A226"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4104,74 +4105,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="43"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="38"/>
       <c r="N1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="44" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="44" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="39" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="18" t="s">
         <v>8</v>
       </c>
@@ -4184,7 +4185,7 @@
       <c r="K3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="45"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:20" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
@@ -4985,74 +4986,78 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="36">
+      <c r="A25" s="48">
         <v>11</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="38" t="s">
+      <c r="B25" s="48" t="s">
+        <v>895</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="48" t="s">
         <v>424</v>
       </c>
-      <c r="H25" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L25" s="40" t="s">
+      <c r="H25" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="52" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="36">
+      <c r="A26" s="48">
         <v>12</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="38" t="s">
+      <c r="B26" s="48" t="s">
+        <v>896</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="H26" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" s="40" t="s">
+      <c r="H26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="52" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>